<commit_message>
Shipper Contact code Updated
</commit_message>
<xml_diff>
--- a/TestData/ShipperContact.xlsx
+++ b/TestData/ShipperContact.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -105,31 +105,31 @@
     <t>AutomationTest</t>
   </si>
   <si>
-    <t>AutomationTest_1014043816</t>
-  </si>
-  <si>
     <t>Name;Email;Phone;Status;</t>
   </si>
   <si>
     <t>automationtest11@gmail.com</t>
   </si>
   <si>
-    <t>AutomationTest_1014052404</t>
-  </si>
-  <si>
-    <t>AutomationTest_1014052553</t>
-  </si>
-  <si>
-    <t>AutomationTest_1014052810</t>
-  </si>
-  <si>
-    <t>AutomationTest_1014053731</t>
-  </si>
-  <si>
-    <t>AutomationTest_1014055224</t>
-  </si>
-  <si>
-    <t>AutomationTest_1014060112</t>
+    <t>AutomationTest_1015094619</t>
+  </si>
+  <si>
+    <t>VERIFY</t>
+  </si>
+  <si>
+    <t>AutomationTest_1015100430</t>
+  </si>
+  <si>
+    <t>AutomationTest_1015100840</t>
+  </si>
+  <si>
+    <t>AutomationTest_1015101850</t>
+  </si>
+  <si>
+    <t>AutomationTest_1015102117</t>
+  </si>
+  <si>
+    <t>AutomationTest_1015102405</t>
   </si>
 </sst>
 </file>
@@ -268,7 +268,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,7 +303,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -628,7 +628,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -644,10 +644,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +702,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>27</v>
@@ -730,7 +730,7 @@
         <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>27</v>
@@ -758,7 +758,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>27</v>
@@ -777,6 +777,32 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>